<commit_message>
New three part level.
</commit_message>
<xml_diff>
--- a/Levels.xlsx
+++ b/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Femto-v0.1.2\projects\RogueBoy_Pokitto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F93F6E7-818E-4DB9-BA07-5688548967B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A587EB3F-5075-4EBF-8F9D-661B07A96D69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="170" yWindow="1550" windowWidth="19180" windowHeight="10180" activeTab="1" xr2:uid="{5767BE84-CE79-9349-AEBF-C6B4E4C3D92E}"/>
+    <workbookView xWindow="1420" yWindow="2090" windowWidth="19180" windowHeight="10180" xr2:uid="{5767BE84-CE79-9349-AEBF-C6B4E4C3D92E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
   <si>
     <t>x</t>
   </si>
@@ -67,18 +67,12 @@
     <t>  // 0</t>
   </si>
   <si>
-    <t>    29</t>
-  </si>
-  <si>
     <t> 0</t>
   </si>
   <si>
     <t>  // 1</t>
   </si>
   <si>
-    <t>    21</t>
-  </si>
-  <si>
     <t>  // 2</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t>  // 7</t>
-  </si>
-  <si>
-    <t>    31</t>
   </si>
   <si>
     <t>  // 8</t>
@@ -489,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26877685-76DE-E24D-ABD4-9D5C27628923}">
   <dimension ref="A1:BK42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -666,39 +657,6 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>0</v>
-      </c>
       <c r="AZ3" s="2"/>
       <c r="BJ3" s="2"/>
     </row>
@@ -706,24 +664,6 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>0</v>
-      </c>
       <c r="AZ4" s="2"/>
       <c r="BJ4" s="2"/>
     </row>
@@ -731,66 +671,6 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" t="s">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>0</v>
-      </c>
       <c r="AZ5" s="2"/>
       <c r="BJ5" s="2"/>
     </row>
@@ -798,12 +678,6 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
       <c r="I6" t="s">
         <v>0</v>
       </c>
@@ -811,24 +685,6 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" t="s">
-        <v>0</v>
-      </c>
-      <c r="W6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="s">
         <v>0</v>
       </c>
       <c r="AZ6" s="2"/>
@@ -838,10 +694,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="s">
+      <c r="H7" t="s">
         <v>0</v>
       </c>
       <c r="AZ7" s="2"/>
@@ -851,43 +704,10 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>0</v>
-      </c>
       <c r="K8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" t="s">
-        <v>0</v>
-      </c>
-      <c r="W8" t="s">
-        <v>0</v>
-      </c>
-      <c r="X8" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="s">
         <v>0</v>
       </c>
       <c r="AZ8" s="2"/>
@@ -897,58 +717,10 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
       <c r="F9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
       <c r="K9" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="s">
         <v>0</v>
       </c>
       <c r="AZ9" s="2"/>
@@ -958,22 +730,10 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="s">
+      <c r="K10" t="s">
         <v>0</v>
       </c>
       <c r="AZ10" s="2"/>
@@ -983,31 +743,19 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
       <c r="F11" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="I11" t="s">
         <v>0</v>
       </c>
-      <c r="R11" t="s">
+      <c r="J11" t="s">
         <v>0</v>
       </c>
-      <c r="S11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="s">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
       <c r="AZ11" s="2"/>
@@ -1181,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B7F1B6-BB46-44F1-B5FC-598D4C1064EA}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:V10"/>
     </sheetView>
   </sheetViews>
@@ -1200,56 +948,56 @@
         <v>38</v>
       </c>
       <c r="C2">
+        <v>38</v>
+      </c>
+      <c r="D2">
         <v>29</v>
       </c>
-      <c r="D2">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
+      <c r="E2">
+        <v>24</v>
       </c>
       <c r="F2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="H2">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I2">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
       <c r="M2">
         <f>I2</f>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="N2">
         <f>H2</f>
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="O2">
         <f>G2</f>
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="P2">
         <f>F2</f>
-        <v>23</v>
-      </c>
-      <c r="Q2" t="str">
+        <v>24</v>
+      </c>
+      <c r="Q2">
         <f>E2</f>
-        <v> 0</v>
+        <v>24</v>
       </c>
       <c r="R2">
         <f>D2</f>
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="S2">
         <f>C2</f>
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="T2">
         <f>B2</f>
@@ -1271,44 +1019,44 @@
         <v>38</v>
       </c>
       <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <v>38</v>
-      </c>
-      <c r="H3">
-        <v>38</v>
-      </c>
-      <c r="I3">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
       </c>
       <c r="M3">
         <f>I3</f>
-        <v>38</v>
-      </c>
-      <c r="N3">
+        <v>23</v>
+      </c>
+      <c r="N3" t="str">
         <f>H3</f>
-        <v>38</v>
-      </c>
-      <c r="O3">
+        <v> 0</v>
+      </c>
+      <c r="O3" t="str">
         <f>G3</f>
-        <v>38</v>
-      </c>
-      <c r="P3">
+        <v> 0</v>
+      </c>
+      <c r="P3" t="str">
         <f>F3</f>
-        <v>23</v>
+        <v> 0</v>
       </c>
       <c r="Q3" t="str">
         <f>E3</f>
@@ -1316,11 +1064,11 @@
       </c>
       <c r="R3">
         <f>D3</f>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="S3">
         <f>C3</f>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="T3">
         <f>B3</f>
@@ -1331,63 +1079,63 @@
         <v>    38</v>
       </c>
       <c r="V3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>24</v>
       </c>
       <c r="D4">
-        <v>48</v>
-      </c>
-      <c r="E4">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="G4">
-        <v>51</v>
-      </c>
-      <c r="H4">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M10" si="0">I4</f>
-        <v>30</v>
-      </c>
-      <c r="N4">
+        <v>23</v>
+      </c>
+      <c r="N4" t="str">
         <f t="shared" ref="N4:N10" si="1">H4</f>
-        <v>24</v>
+        <v> 0</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O10" si="2">G4</f>
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P10" si="3">F4</f>
-        <v>34</v>
-      </c>
-      <c r="Q4">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="str">
         <f t="shared" ref="Q4:Q10" si="4">E4</f>
-        <v>59</v>
+        <v> 0</v>
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R10" si="5">D4</f>
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S10" si="6">C4</f>
@@ -1395,58 +1143,58 @@
       </c>
       <c r="T4">
         <f t="shared" ref="T4:T10" si="7">B4</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="U4" t="str">
         <f t="shared" ref="U4:U10" si="8">A4</f>
-        <v>    29</v>
+        <v>    38</v>
       </c>
       <c r="V4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>46</v>
-      </c>
-      <c r="H5">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
         <v>11</v>
       </c>
       <c r="I5">
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="str">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v> 0</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="3"/>
@@ -1466,46 +1214,46 @@
       </c>
       <c r="T5">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="U5" t="str">
         <f t="shared" si="8"/>
-        <v>    21</v>
+        <v>    38</v>
       </c>
       <c r="V5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -1517,7 +1265,7 @@
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="3"/>
@@ -1537,37 +1285,37 @@
       </c>
       <c r="T6">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="8"/>
-        <v>    21</v>
+        <v>    38</v>
       </c>
       <c r="V6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H7">
         <v>22</v>
@@ -1576,7 +1324,7 @@
         <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
@@ -1588,7 +1336,7 @@
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="3"/>
@@ -1608,37 +1356,37 @@
       </c>
       <c r="T7">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="8"/>
-        <v>    21</v>
+        <v>    38</v>
       </c>
       <c r="V7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>22</v>
       </c>
       <c r="D8">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E8">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="G8">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H8">
         <v>38</v>
@@ -1647,7 +1395,7 @@
         <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
@@ -1659,19 +1407,19 @@
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="P8">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="Q8">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="R8">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="S8">
         <f t="shared" si="6"/>
@@ -1679,14 +1427,14 @@
       </c>
       <c r="T8">
         <f t="shared" si="7"/>
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="8"/>
-        <v>    31</v>
+        <v>    38</v>
       </c>
       <c r="V8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -1700,16 +1448,16 @@
         <v>38</v>
       </c>
       <c r="D9">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="E9">
+        <v>38</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="G9">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H9">
         <v>38</v>
@@ -1718,7 +1466,7 @@
         <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
@@ -1730,19 +1478,19 @@
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="P9">
         <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="Q9" t="str">
+        <v>38</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="4"/>
-        <v> 0</v>
+        <v>38</v>
       </c>
       <c r="R9">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="S9">
         <f t="shared" si="6"/>
@@ -1757,7 +1505,7 @@
         <v>    38</v>
       </c>
       <c r="V9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
@@ -1771,16 +1519,16 @@
         <v>38</v>
       </c>
       <c r="D10">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="E10">
+        <v>38</v>
       </c>
       <c r="F10">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>38</v>
@@ -1789,7 +1537,7 @@
         <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
@@ -1801,19 +1549,19 @@
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="P10">
         <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="Q10" t="str">
+        <v>38</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="4"/>
-        <v> 0</v>
+        <v>38</v>
       </c>
       <c r="R10">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="S10">
         <f t="shared" si="6"/>
@@ -1828,7 +1576,7 @@
         <v>    38</v>
       </c>
       <c r="V10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before changing corner fill logic.
</commit_message>
<xml_diff>
--- a/Levels.xlsx
+++ b/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Femto-v0.1.2\projects\RogueBoy_Pokitto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A587EB3F-5075-4EBF-8F9D-661B07A96D69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20D5B1A-BD89-49AD-862D-07818659A185}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="2090" windowWidth="19180" windowHeight="10180" xr2:uid="{5767BE84-CE79-9349-AEBF-C6B4E4C3D92E}"/>
+    <workbookView xWindow="-50" yWindow="1980" windowWidth="19180" windowHeight="10180" xr2:uid="{5767BE84-CE79-9349-AEBF-C6B4E4C3D92E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="29">
   <si>
     <t>x</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t>  // 8</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -481,12 +508,13 @@
   <dimension ref="A1:BK42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="3.1640625" style="1"/>
+    <col min="10" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" style="2"/>
     <col min="22" max="22" width="3.1640625" style="2"/>
     <col min="32" max="32" width="3.1640625" style="2"/>
@@ -495,85 +523,85 @@
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.35">
       <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>6</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>7</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>8</v>
       </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
       <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
         <v>1</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>3</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>4</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>5</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>6</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>7</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>8</v>
       </c>
-      <c r="U1">
-        <v>9</v>
-      </c>
       <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1">
         <v>1</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>2</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>3</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>4</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>5</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>6</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>7</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>8</v>
-      </c>
-      <c r="AE1">
-        <v>9</v>
       </c>
       <c r="AG1">
         <v>1</v>
@@ -655,36 +683,246 @@
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>0</v>
       </c>
       <c r="AZ3" s="2"/>
       <c r="BJ3" s="2"/>
     </row>
     <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>0</v>
       </c>
       <c r="AZ4" s="2"/>
       <c r="BJ4" s="2"/>
     </row>
     <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>0</v>
       </c>
       <c r="AZ5" s="2"/>
       <c r="BJ5" s="2"/>
     </row>
     <row r="6" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
         <v>0</v>
       </c>
       <c r="AZ6" s="2"/>
@@ -692,22 +930,73 @@
     </row>
     <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="W7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>25</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BJ7" s="2"/>
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
-      <c r="K8" t="s">
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="s">
         <v>0</v>
       </c>
       <c r="AZ8" s="2"/>
@@ -715,12 +1004,54 @@
     </row>
     <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
         <v>0</v>
       </c>
       <c r="K9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE9" t="s">
         <v>0</v>
       </c>
       <c r="AZ9" s="2"/>
@@ -728,12 +1059,54 @@
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE10" t="s">
         <v>0</v>
       </c>
       <c r="AZ10" s="2"/>
@@ -741,11 +1114,23 @@
     </row>
     <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
       </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
       <c r="H11" t="s">
         <v>0</v>
       </c>
@@ -756,6 +1141,60 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="s">
         <v>0</v>
       </c>
       <c r="AZ11" s="2"/>
@@ -771,10 +1210,145 @@
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <v>12</v>
+      </c>
+      <c r="Q13">
+        <v>13</v>
+      </c>
+      <c r="R13">
+        <v>14</v>
+      </c>
+      <c r="S13">
+        <v>15</v>
+      </c>
+      <c r="T13">
+        <v>16</v>
+      </c>
+      <c r="U13">
+        <v>17</v>
+      </c>
+      <c r="W13">
+        <v>18</v>
+      </c>
+      <c r="X13">
+        <v>19</v>
+      </c>
+      <c r="Y13">
+        <v>20</v>
+      </c>
+      <c r="Z13">
+        <v>21</v>
+      </c>
+      <c r="AA13">
+        <v>22</v>
+      </c>
+      <c r="AB13">
+        <v>23</v>
+      </c>
+      <c r="AC13">
+        <v>24</v>
+      </c>
+      <c r="AD13">
+        <v>25</v>
+      </c>
+      <c r="AE13">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
+      </c>
+      <c r="C14">
+        <v>-18</v>
+      </c>
+      <c r="D14">
+        <v>-17</v>
+      </c>
+      <c r="E14">
+        <v>-16</v>
+      </c>
+      <c r="F14">
+        <v>-15</v>
+      </c>
+      <c r="G14">
+        <v>-14</v>
+      </c>
+      <c r="H14">
+        <v>-13</v>
+      </c>
+      <c r="I14">
+        <v>-12</v>
+      </c>
+      <c r="J14">
+        <v>-11</v>
+      </c>
+      <c r="K14">
+        <v>-10</v>
+      </c>
+      <c r="M14">
+        <v>-9</v>
+      </c>
+      <c r="N14">
+        <v>-8</v>
+      </c>
+      <c r="O14">
+        <v>-7</v>
+      </c>
+      <c r="P14">
+        <v>-6</v>
+      </c>
+      <c r="Q14">
+        <v>-5</v>
+      </c>
+      <c r="R14">
+        <v>-4</v>
+      </c>
+      <c r="S14">
+        <v>-3</v>
+      </c>
+      <c r="T14">
+        <v>-2</v>
+      </c>
+      <c r="U14">
+        <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:63" x14ac:dyDescent="0.35">

</xml_diff>